<commit_message>
update daily incidence data
</commit_message>
<xml_diff>
--- a/data/covid19/daily_confirmed_total.xlsx
+++ b/data/covid19/daily_confirmed_total.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/covid19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/covid19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{381AF413-F532-CE4C-9F3A-70CD24887259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB8F450-7C5C-8849-BD8A-D526F92A784D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11240" yWindow="1480" windowWidth="27240" windowHeight="14800" xr2:uid="{CDB7026C-D039-6E42-A7EC-DD15752F5A04}"/>
+    <workbookView xWindow="5000" yWindow="2720" windowWidth="27240" windowHeight="14800" xr2:uid="{CDB7026C-D039-6E42-A7EC-DD15752F5A04}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_confirmed_total" sheetId="3" r:id="rId1"/>
     <sheet name="Gyeonggi" sheetId="1" r:id="rId2"/>
     <sheet name="Seoul" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,10 +69,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84E97E4-59A3-2A4A-9E04-1110D78C4BE7}">
-  <dimension ref="A1:J199"/>
+  <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8574,7 +8580,49 @@
         <v>6</v>
       </c>
     </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B200">
+        <f>Gyeonggi!B200+Seoul!B200</f>
+        <v>95</v>
+      </c>
+      <c r="C200">
+        <f>Gyeonggi!C200+Seoul!C200</f>
+        <v>104</v>
+      </c>
+      <c r="D200">
+        <f>Gyeonggi!D200+Seoul!D200</f>
+        <v>296</v>
+      </c>
+      <c r="E200">
+        <f>Gyeonggi!E200+Seoul!E200</f>
+        <v>236</v>
+      </c>
+      <c r="F200">
+        <f>Gyeonggi!F200+Seoul!F200</f>
+        <v>206</v>
+      </c>
+      <c r="G200">
+        <f>Gyeonggi!G200+Seoul!G200</f>
+        <v>189</v>
+      </c>
+      <c r="H200">
+        <f>Gyeonggi!H200+Seoul!H200</f>
+        <v>99</v>
+      </c>
+      <c r="I200">
+        <f>Gyeonggi!I200+Seoul!I200</f>
+        <v>24</v>
+      </c>
+      <c r="J200">
+        <f>Gyeonggi!J200+Seoul!J200</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8583,8 +8631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F15847C-BF25-C644-B62C-91A3E2AC597B}">
   <dimension ref="A1:J562"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="J104" sqref="J104"/>
+    <sheetView topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14955,31 +15003,292 @@
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A200" s="1"/>
+      <c r="A200" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B200">
+        <v>59</v>
+      </c>
+      <c r="C200">
+        <v>65</v>
+      </c>
+      <c r="D200">
+        <v>149</v>
+      </c>
+      <c r="E200">
+        <v>124</v>
+      </c>
+      <c r="F200">
+        <v>128</v>
+      </c>
+      <c r="G200">
+        <v>114</v>
+      </c>
+      <c r="H200">
+        <v>44</v>
+      </c>
+      <c r="I200">
+        <v>9</v>
+      </c>
+      <c r="J200">
+        <v>6</v>
+      </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A201" s="1"/>
+      <c r="A201" s="1">
+        <v>44441</v>
+      </c>
+      <c r="B201">
+        <v>31</v>
+      </c>
+      <c r="C201">
+        <v>48</v>
+      </c>
+      <c r="D201">
+        <v>104</v>
+      </c>
+      <c r="E201">
+        <v>105</v>
+      </c>
+      <c r="F201">
+        <v>96</v>
+      </c>
+      <c r="G201">
+        <v>82</v>
+      </c>
+      <c r="H201">
+        <v>39</v>
+      </c>
+      <c r="I201">
+        <v>7</v>
+      </c>
+      <c r="J201">
+        <v>9</v>
+      </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A202" s="1"/>
+      <c r="A202" s="1">
+        <v>44442</v>
+      </c>
+      <c r="B202">
+        <v>30</v>
+      </c>
+      <c r="C202">
+        <v>45</v>
+      </c>
+      <c r="D202">
+        <v>130</v>
+      </c>
+      <c r="E202">
+        <v>125</v>
+      </c>
+      <c r="F202">
+        <v>106</v>
+      </c>
+      <c r="G202">
+        <v>85</v>
+      </c>
+      <c r="H202">
+        <v>46</v>
+      </c>
+      <c r="I202">
+        <v>11</v>
+      </c>
+      <c r="J202">
+        <v>2</v>
+      </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A203" s="1"/>
+      <c r="A203" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B203">
+        <v>31</v>
+      </c>
+      <c r="C203">
+        <v>44</v>
+      </c>
+      <c r="D203">
+        <v>93</v>
+      </c>
+      <c r="E203">
+        <v>100</v>
+      </c>
+      <c r="F203">
+        <v>81</v>
+      </c>
+      <c r="G203">
+        <v>43</v>
+      </c>
+      <c r="H203">
+        <v>38</v>
+      </c>
+      <c r="I203">
+        <v>14</v>
+      </c>
+      <c r="J203">
+        <v>4</v>
+      </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A204" s="1"/>
+      <c r="A204" s="1">
+        <v>44444</v>
+      </c>
+      <c r="B204">
+        <v>37</v>
+      </c>
+      <c r="C204">
+        <v>51</v>
+      </c>
+      <c r="D204">
+        <v>63</v>
+      </c>
+      <c r="E204">
+        <v>76</v>
+      </c>
+      <c r="F204">
+        <v>69</v>
+      </c>
+      <c r="G204">
+        <v>63</v>
+      </c>
+      <c r="H204">
+        <v>34</v>
+      </c>
+      <c r="I204">
+        <v>8</v>
+      </c>
+      <c r="J204">
+        <v>2</v>
+      </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A205" s="1"/>
+      <c r="A205" s="1">
+        <v>44445</v>
+      </c>
+      <c r="B205">
+        <v>36</v>
+      </c>
+      <c r="C205">
+        <v>40</v>
+      </c>
+      <c r="D205">
+        <v>106</v>
+      </c>
+      <c r="E205">
+        <v>93</v>
+      </c>
+      <c r="F205">
+        <v>103</v>
+      </c>
+      <c r="G205">
+        <v>64</v>
+      </c>
+      <c r="H205">
+        <v>28</v>
+      </c>
+      <c r="I205">
+        <v>8</v>
+      </c>
+      <c r="J205">
+        <v>3</v>
+      </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A206" s="1"/>
+      <c r="A206" s="1">
+        <v>44446</v>
+      </c>
+      <c r="B206">
+        <v>38</v>
+      </c>
+      <c r="C206">
+        <v>79</v>
+      </c>
+      <c r="D206">
+        <v>151</v>
+      </c>
+      <c r="E206">
+        <v>148</v>
+      </c>
+      <c r="F206">
+        <v>126</v>
+      </c>
+      <c r="G206">
+        <v>99</v>
+      </c>
+      <c r="H206">
+        <v>45</v>
+      </c>
+      <c r="I206">
+        <v>12</v>
+      </c>
+      <c r="J206">
+        <v>5</v>
+      </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A207" s="1"/>
+      <c r="A207" s="1">
+        <v>44447</v>
+      </c>
+      <c r="B207">
+        <v>58</v>
+      </c>
+      <c r="C207">
+        <v>70</v>
+      </c>
+      <c r="D207">
+        <v>120</v>
+      </c>
+      <c r="E207">
+        <v>121</v>
+      </c>
+      <c r="F207">
+        <v>129</v>
+      </c>
+      <c r="G207">
+        <v>85</v>
+      </c>
+      <c r="H207">
+        <v>49</v>
+      </c>
+      <c r="I207">
+        <v>8</v>
+      </c>
+      <c r="J207">
+        <v>3</v>
+      </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A208" s="1"/>
+      <c r="A208" s="1">
+        <v>44448</v>
+      </c>
+      <c r="B208">
+        <v>26</v>
+      </c>
+      <c r="C208">
+        <v>53</v>
+      </c>
+      <c r="D208">
+        <v>119</v>
+      </c>
+      <c r="E208">
+        <v>116</v>
+      </c>
+      <c r="F208">
+        <v>120</v>
+      </c>
+      <c r="G208">
+        <v>99</v>
+      </c>
+      <c r="H208">
+        <v>43</v>
+      </c>
+      <c r="I208">
+        <v>14</v>
+      </c>
+      <c r="J208">
+        <v>23</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
@@ -16052,8 +16361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A71476-9D4C-5143-A8A9-0CE4866D48A6}">
   <dimension ref="A1:J565"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="J204" sqref="J204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22400,7 +22709,36 @@
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A200" s="1"/>
+      <c r="A200" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B200">
+        <v>36</v>
+      </c>
+      <c r="C200">
+        <v>39</v>
+      </c>
+      <c r="D200">
+        <v>147</v>
+      </c>
+      <c r="E200">
+        <v>112</v>
+      </c>
+      <c r="F200">
+        <v>78</v>
+      </c>
+      <c r="G200">
+        <v>75</v>
+      </c>
+      <c r="H200">
+        <v>55</v>
+      </c>
+      <c r="I200">
+        <v>15</v>
+      </c>
+      <c r="J200">
+        <v>2</v>
+      </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>

</xml_diff>